<commit_message>
add test data for overtemp
</commit_message>
<xml_diff>
--- a/cmd/dynamic_temp.xlsx
+++ b/cmd/dynamic_temp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyrila/work/smarthome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyrila/.config/homekit.sh/accessories/stiebel/cmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6329F3C2-7225-4449-8A6B-1C14F2E042A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717B2E2E-716A-C641-AC70-72703EB24B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{F4BD59F9-C06B-BE42-B981-3B273D8F5AA5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>price</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>room_18</t>
+  </si>
+  <si>
+    <t>room_22</t>
   </si>
 </sst>
 </file>
@@ -190,8 +193,147 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>22</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AE68-0F44-8930-BDEB62F61131}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>21</c:v>
           </c:tx>
@@ -323,102 +465,102 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$C$2:$C$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>23.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.0205999132796</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.559319556497201</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.4678748622465</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.596373105057499</c:v>
+                  <c:v>17.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.8708664335714</c:v>
+                  <c:v>16.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.2493873660829</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.705810742857</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.222763947111499</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.7881070093006</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.3930215964638</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.030899869919399</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>15.696662315049901</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.386319977650199</c:v>
+                  <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.096683018297</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.825160557860899</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.569619513137001</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.328282715969801</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.099653886374799</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13.882461389442399</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.675615400843901</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.4781748188863</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.289321377282601</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13.108339156354599</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.934598195660399</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.7675412606319</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>12.6066730616973</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.4515513999148</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12.3017798402183</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12.1570016065321</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12.016894462103901</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -432,7 +574,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>20</c:v>
           </c:tx>
@@ -564,102 +706,102 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$32</c:f>
+              <c:f>Sheet1!$D$2:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.0205999132796</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.559319556497201</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.4678748622465</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.596373105057499</c:v>
+                  <c:v>19.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.8708664335714</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.2493873660829</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.705810742857</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.222763947111499</c:v>
+                  <c:v>17.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17.7881070093006</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.3930215964638</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.030899869919399</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.696662315049899</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16.386319977650199</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.096683018297</c:v>
+                  <c:v>15.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.825160557860899</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.569619513137001</c:v>
+                  <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.328282715969801</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15.099653886374799</c:v>
+                  <c:v>14.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.882461389442399</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.675615400843901</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14.4781748188863</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14.289321377282601</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.108339156354599</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13.934598195660399</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13.7675412606319</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.6066730616973</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.4515513999148</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13.3017798402183</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.1570016065321</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>13.016894462103901</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,7 +815,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>19</c:v>
           </c:tx>
@@ -805,102 +947,102 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$32</c:f>
+              <c:f>Sheet1!$E$2:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0205999132796</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.559319556497201</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.4678748622465</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.596373105057499</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.8708664335714</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.2493873660829</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.705810742857</c:v>
+                  <c:v>19.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.222763947111499</c:v>
+                  <c:v>19.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.7881070093006</c:v>
+                  <c:v>18.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.3930215964638</c:v>
+                  <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.030899869919399</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.696662315049899</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.386319977650199</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.096683018297</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.825160557860901</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.569619513136999</c:v>
+                  <c:v>16.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16.328282715969799</c:v>
+                  <c:v>16.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.099653886374799</c:v>
+                  <c:v>16.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15.882461389442399</c:v>
+                  <c:v>15.9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>15.675615400843901</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15.4781748188863</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15.289321377282601</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15.108339156354599</c:v>
+                  <c:v>15.1</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.934598195660399</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.7675412606319</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>14.6066730616973</c:v>
+                  <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14.4515513999148</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14.3017798402183</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14.1570016065321</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.016894462103901</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,7 +1056,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>18</c:v>
           </c:tx>
@@ -1046,102 +1188,102 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$32</c:f>
+              <c:f>Sheet1!$F$2:$F$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0205999132796</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.559319556497201</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.4678748622465</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.596373105057499</c:v>
+                  <c:v>23.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.8708664335714</c:v>
+                  <c:v>22.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.2493873660829</c:v>
+                  <c:v>22.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.705810742857</c:v>
+                  <c:v>21.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.222763947111499</c:v>
+                  <c:v>21.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.7881070093006</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.3930215964638</c:v>
+                  <c:v>20.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.030899869919399</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.696662315049899</c:v>
+                  <c:v>19.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.386319977650199</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.096683018297</c:v>
+                  <c:v>19.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.825160557860901</c:v>
+                  <c:v>18.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.569619513136999</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.328282715969799</c:v>
+                  <c:v>18.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.099653886374799</c:v>
+                  <c:v>18.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16.882461389442401</c:v>
+                  <c:v>17.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.675615400843899</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>16.478174818886298</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16.289321377282601</c:v>
+                  <c:v>17.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>16.108339156354599</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15.934598195660399</c:v>
+                  <c:v>16.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>15.7675412606319</c:v>
+                  <c:v>16.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15.6066730616973</c:v>
+                  <c:v>16.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15.4515513999148</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15.3017798402183</c:v>
+                  <c:v>16.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.1570016065321</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15.016894462103901</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,13 +2187,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -2083,9 +2225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2123,7 +2265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2229,7 +2371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2371,7 +2513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2379,556 +2521,656 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA4EFB9-26F4-D54F-AF75-7A97135D06EC}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
+        <v>21.2</v>
+      </c>
+      <c r="C2" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="D2" s="3">
         <v>25</v>
       </c>
-      <c r="C2" s="3">
-        <v>26</v>
-      </c>
-      <c r="D2" s="3">
-        <v>27</v>
-      </c>
       <c r="E2" s="3">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="F2" s="3">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
-        <v>23.0205999132796</v>
+      <c r="B3" s="2">
+        <v>19</v>
       </c>
       <c r="C3" s="3">
-        <v>24.0205999132796</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3">
-        <v>25.0205999132796</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3">
-        <v>26.0205999132796</v>
+        <v>25</v>
+      </c>
+      <c r="F3" s="3">
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>21.559319556497201</v>
+      <c r="B4" s="2">
+        <v>17.600000000000001</v>
       </c>
       <c r="C4" s="3">
-        <v>22.559319556497201</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="D4" s="3">
-        <v>23.559319556497201</v>
+        <v>21.6</v>
       </c>
       <c r="E4" s="3">
-        <v>24.559319556497201</v>
+        <v>23.6</v>
+      </c>
+      <c r="F4" s="3">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>20.4678748622465</v>
+      <c r="B5" s="2">
+        <v>16.5</v>
       </c>
       <c r="C5" s="3">
-        <v>21.4678748622465</v>
+        <v>18.5</v>
       </c>
       <c r="D5" s="3">
-        <v>22.4678748622465</v>
+        <v>20.5</v>
       </c>
       <c r="E5" s="3">
-        <v>23.4678748622465</v>
+        <v>22.5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>24.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>19.596373105057499</v>
+      <c r="B6" s="2">
+        <v>15.6</v>
       </c>
       <c r="C6" s="3">
-        <v>20.596373105057499</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="D6" s="3">
-        <v>21.596373105057499</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E6" s="3">
-        <v>22.596373105057499</v>
+        <v>21.6</v>
+      </c>
+      <c r="F6" s="3">
+        <v>23.6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>18.8708664335714</v>
+      <c r="B7" s="2">
+        <v>14.9</v>
       </c>
       <c r="C7" s="3">
-        <v>19.8708664335714</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>20.8708664335714</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E7" s="3">
-        <v>21.8708664335714</v>
+        <v>20.9</v>
+      </c>
+      <c r="F7" s="3">
+        <v>22.9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>18.2493873660829</v>
+      <c r="B8" s="2">
+        <v>14.2</v>
       </c>
       <c r="C8" s="3">
-        <v>19.2493873660829</v>
+        <v>16.2</v>
       </c>
       <c r="D8" s="3">
-        <v>20.2493873660829</v>
+        <v>18.2</v>
       </c>
       <c r="E8" s="3">
-        <v>21.2493873660829</v>
+        <v>20.2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>22.2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>17.705810742857</v>
+      <c r="B9" s="2">
+        <v>13.7</v>
       </c>
       <c r="C9" s="3">
-        <v>18.705810742857</v>
+        <v>15.7</v>
       </c>
       <c r="D9" s="3">
-        <v>19.705810742857</v>
+        <v>17.7</v>
       </c>
       <c r="E9" s="3">
-        <v>20.705810742857</v>
+        <v>19.7</v>
+      </c>
+      <c r="F9" s="3">
+        <v>21.7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>17.222763947111499</v>
+      <c r="B10" s="2">
+        <v>13.2</v>
       </c>
       <c r="C10" s="3">
-        <v>18.222763947111499</v>
+        <v>15.2</v>
       </c>
       <c r="D10" s="3">
-        <v>19.222763947111499</v>
+        <v>17.2</v>
       </c>
       <c r="E10" s="3">
-        <v>20.222763947111499</v>
+        <v>19.2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>21.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>16.7881070093006</v>
+      <c r="B11" s="2">
+        <v>12.8</v>
       </c>
       <c r="C11" s="3">
-        <v>17.7881070093006</v>
+        <v>14.8</v>
       </c>
       <c r="D11" s="3">
-        <v>18.7881070093006</v>
+        <v>16.8</v>
       </c>
       <c r="E11" s="3">
-        <v>19.7881070093006</v>
+        <v>18.8</v>
+      </c>
+      <c r="F11" s="3">
+        <v>20.8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>16.3930215964638</v>
+      <c r="B12" s="2">
+        <v>12.4</v>
       </c>
       <c r="C12" s="3">
-        <v>17.3930215964638</v>
+        <v>14.4</v>
       </c>
       <c r="D12" s="3">
-        <v>18.3930215964638</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="E12" s="3">
-        <v>19.3930215964638</v>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>16.030899869919399</v>
+      <c r="B13" s="2">
+        <v>12</v>
       </c>
       <c r="C13" s="3">
-        <v>17.030899869919399</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3">
-        <v>18.030899869919399</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3">
-        <v>19.030899869919399</v>
+        <v>18</v>
+      </c>
+      <c r="F13" s="3">
+        <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>15.696662315049901</v>
+      <c r="B14" s="2">
+        <v>12</v>
       </c>
       <c r="C14" s="3">
-        <v>16.696662315049899</v>
+        <v>13.7</v>
       </c>
       <c r="D14" s="3">
-        <v>17.696662315049899</v>
+        <v>15.7</v>
       </c>
       <c r="E14" s="3">
-        <v>18.696662315049899</v>
+        <v>17.7</v>
+      </c>
+      <c r="F14" s="3">
+        <v>19.7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>15.386319977650199</v>
+      <c r="B15" s="2">
+        <v>12</v>
       </c>
       <c r="C15" s="3">
-        <v>16.386319977650199</v>
+        <v>13.4</v>
       </c>
       <c r="D15" s="3">
-        <v>17.386319977650199</v>
+        <v>15.4</v>
       </c>
       <c r="E15" s="3">
-        <v>18.386319977650199</v>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>15.096683018297</v>
+      <c r="B16" s="2">
+        <v>12</v>
       </c>
       <c r="C16" s="3">
-        <v>16.096683018297</v>
+        <v>13.1</v>
       </c>
       <c r="D16" s="3">
-        <v>17.096683018297</v>
+        <v>15.1</v>
       </c>
       <c r="E16" s="3">
-        <v>18.096683018297</v>
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F16" s="3">
+        <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>14.825160557860899</v>
+      <c r="B17" s="2">
+        <v>12</v>
       </c>
       <c r="C17" s="3">
-        <v>15.825160557860899</v>
+        <v>12.8</v>
       </c>
       <c r="D17" s="3">
-        <v>16.825160557860901</v>
+        <v>14.8</v>
       </c>
       <c r="E17" s="3">
-        <v>17.825160557860901</v>
+        <v>16.8</v>
+      </c>
+      <c r="F17" s="3">
+        <v>18.8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>14.569619513137001</v>
+      <c r="B18" s="2">
+        <v>12</v>
       </c>
       <c r="C18" s="3">
-        <v>15.569619513137001</v>
+        <v>12.6</v>
       </c>
       <c r="D18" s="3">
-        <v>16.569619513136999</v>
+        <v>14.6</v>
       </c>
       <c r="E18" s="3">
-        <v>17.569619513136999</v>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F18" s="3">
+        <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <v>14.328282715969801</v>
+      <c r="B19" s="2">
+        <v>12</v>
       </c>
       <c r="C19" s="3">
-        <v>15.328282715969801</v>
+        <v>12.3</v>
       </c>
       <c r="D19" s="3">
-        <v>16.328282715969799</v>
+        <v>14.3</v>
       </c>
       <c r="E19" s="3">
-        <v>17.328282715969799</v>
+        <v>16.3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>18.3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <v>14.099653886374799</v>
+      <c r="B20" s="2">
+        <v>12</v>
       </c>
       <c r="C20" s="3">
-        <v>15.099653886374799</v>
+        <v>12.1</v>
       </c>
       <c r="D20" s="3">
-        <v>16.099653886374799</v>
+        <v>14.1</v>
       </c>
       <c r="E20" s="3">
-        <v>17.099653886374799</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F20" s="3">
+        <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <v>13.882461389442399</v>
+      <c r="B21" s="2">
+        <v>12</v>
       </c>
       <c r="C21" s="3">
-        <v>14.882461389442399</v>
+        <v>12</v>
       </c>
       <c r="D21" s="3">
-        <v>15.882461389442399</v>
+        <v>13.9</v>
       </c>
       <c r="E21" s="3">
-        <v>16.882461389442401</v>
+        <v>15.9</v>
+      </c>
+      <c r="F21" s="3">
+        <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <v>13.675615400843901</v>
+      <c r="B22" s="2">
+        <v>12</v>
       </c>
       <c r="C22" s="3">
-        <v>14.675615400843901</v>
+        <v>12</v>
       </c>
       <c r="D22" s="3">
-        <v>15.675615400843901</v>
+        <v>13.7</v>
       </c>
       <c r="E22" s="3">
-        <v>16.675615400843899</v>
+        <v>15.7</v>
+      </c>
+      <c r="F22" s="3">
+        <v>17.7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <v>13.4781748188863</v>
+      <c r="B23" s="2">
+        <v>12</v>
       </c>
       <c r="C23" s="3">
-        <v>14.4781748188863</v>
+        <v>12</v>
       </c>
       <c r="D23" s="3">
-        <v>15.4781748188863</v>
+        <v>13.5</v>
       </c>
       <c r="E23" s="3">
-        <v>16.478174818886298</v>
+        <v>15.5</v>
+      </c>
+      <c r="F23" s="3">
+        <v>17.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <v>13.289321377282601</v>
+      <c r="B24" s="2">
+        <v>12</v>
       </c>
       <c r="C24" s="3">
-        <v>14.289321377282601</v>
+        <v>12</v>
       </c>
       <c r="D24" s="3">
-        <v>15.289321377282601</v>
+        <v>13.3</v>
       </c>
       <c r="E24" s="3">
-        <v>16.289321377282601</v>
+        <v>15.3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>17.3</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <v>13.108339156354599</v>
+      <c r="B25" s="2">
+        <v>12</v>
       </c>
       <c r="C25" s="3">
-        <v>14.108339156354599</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3">
-        <v>15.108339156354599</v>
+        <v>13.1</v>
       </c>
       <c r="E25" s="3">
-        <v>16.108339156354599</v>
+        <v>15.1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
-        <v>12.934598195660399</v>
+      <c r="B26" s="2">
+        <v>12</v>
       </c>
       <c r="C26" s="3">
-        <v>13.934598195660399</v>
+        <v>12</v>
       </c>
       <c r="D26" s="3">
-        <v>14.934598195660399</v>
+        <v>12.9</v>
       </c>
       <c r="E26" s="3">
-        <v>15.934598195660399</v>
+        <v>14.9</v>
+      </c>
+      <c r="F26" s="3">
+        <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
-        <v>12.7675412606319</v>
+      <c r="B27" s="2">
+        <v>12</v>
       </c>
       <c r="C27" s="3">
-        <v>13.7675412606319</v>
+        <v>12</v>
       </c>
       <c r="D27" s="3">
-        <v>14.7675412606319</v>
+        <v>12.8</v>
       </c>
       <c r="E27" s="3">
-        <v>15.7675412606319</v>
+        <v>14.8</v>
+      </c>
+      <c r="F27" s="3">
+        <v>16.8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
-        <v>12.6066730616973</v>
+      <c r="B28" s="2">
+        <v>12</v>
       </c>
       <c r="C28" s="3">
-        <v>13.6066730616973</v>
+        <v>12</v>
       </c>
       <c r="D28" s="3">
-        <v>14.6066730616973</v>
+        <v>12.6</v>
       </c>
       <c r="E28" s="3">
-        <v>15.6066730616973</v>
+        <v>14.6</v>
+      </c>
+      <c r="F28" s="3">
+        <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
-        <v>12.4515513999148</v>
+      <c r="B29" s="2">
+        <v>12</v>
       </c>
       <c r="C29" s="3">
-        <v>13.4515513999148</v>
+        <v>12</v>
       </c>
       <c r="D29" s="3">
-        <v>14.4515513999148</v>
+        <v>12.5</v>
       </c>
       <c r="E29" s="3">
-        <v>15.4515513999148</v>
+        <v>14.5</v>
+      </c>
+      <c r="F29" s="3">
+        <v>16.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
-        <v>12.3017798402183</v>
+      <c r="B30" s="2">
+        <v>12</v>
       </c>
       <c r="C30" s="3">
-        <v>13.3017798402183</v>
+        <v>12</v>
       </c>
       <c r="D30" s="3">
-        <v>14.3017798402183</v>
+        <v>12.3</v>
       </c>
       <c r="E30" s="3">
-        <v>15.3017798402183</v>
+        <v>14.3</v>
+      </c>
+      <c r="F30" s="3">
+        <v>16.3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
-        <v>12.1570016065321</v>
+      <c r="B31" s="2">
+        <v>12</v>
       </c>
       <c r="C31" s="3">
-        <v>13.1570016065321</v>
+        <v>12</v>
       </c>
       <c r="D31" s="3">
-        <v>14.1570016065321</v>
+        <v>12.2</v>
       </c>
       <c r="E31" s="3">
-        <v>15.1570016065321</v>
+        <v>14.2</v>
+      </c>
+      <c r="F31" s="3">
+        <v>16.2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="3">
-        <v>12.016894462103901</v>
+      <c r="B32" s="2">
+        <v>12</v>
       </c>
       <c r="C32" s="3">
-        <v>13.016894462103901</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3">
-        <v>14.016894462103901</v>
+        <v>12</v>
       </c>
       <c r="E32" s="3">
-        <v>15.016894462103901</v>
+        <v>14</v>
+      </c>
+      <c r="F32" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>